<commit_message>
Sending emails through Python
Sending emails through python now. Wow. I can code, but I'm hella unorganized in it.
</commit_message>
<xml_diff>
--- a/Outreach - Skyscraper/Output/Current/wfh.xlsx
+++ b/Outreach - Skyscraper/Output/Current/wfh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hooman Deghani\Python\Data Analysis\Outreach - Skyscraper\Output\Current\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E765033-6A73-405F-88DB-D17EAA6FD7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F13CAD6-2430-4361-B291-49ABBB30883D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14077,11 +14077,12 @@
   <dimension ref="A1:M1515"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.5703125" customWidth="1"/>

</xml_diff>